<commit_message>
Últimos ajustes nos artefatos
</commit_message>
<xml_diff>
--- a/Artefatos/23. Matrizes de rastreabilidade (Caracteristicas x SSS_ Incompleto).xlsx
+++ b/Artefatos/23. Matrizes de rastreabilidade (Caracteristicas x SSS_ Incompleto).xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive\Área de Trabalho\GIT\OPE-Madara\Artefatos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70942807-F1E9-45A2-A430-2FFC83E200C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="65">
   <si>
     <t>CAR 0001</t>
   </si>
@@ -203,42 +212,62 @@
   </si>
   <si>
     <t>SSS-0014</t>
+  </si>
+  <si>
+    <t>Matrizes de Rastreabilidade(Características X SSS)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -252,9 +281,27 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -268,41 +315,57 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -492,303 +555,250 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AX16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B1" sqref="B1" pane="topRight"/>
-      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
-      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.86"/>
-    <col customWidth="1" min="2" max="50" width="10.0"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="50" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:50" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7"/>
+      <c r="B1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="1"/>
+    </row>
+    <row r="2" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AV2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AW2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="4"/>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3"/>
-      <c r="AQ2" s="3"/>
-      <c r="AR2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS2" s="3"/>
-      <c r="AT2" s="3"/>
-      <c r="AU2" s="3"/>
-      <c r="AV2" s="3"/>
-      <c r="AW2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -812,12 +822,8 @@
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
-      <c r="V3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
       <c r="X3" s="3" t="s">
         <v>50</v>
       </c>
@@ -851,19 +857,17 @@
       <c r="AH3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AI3" s="3"/>
+      <c r="AI3" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="AJ3" s="3" t="s">
         <v>50</v>
       </c>
       <c r="AK3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AL3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
       <c r="AN3" s="4"/>
       <c r="AO3" s="3"/>
       <c r="AP3" s="3"/>
@@ -882,9 +886,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>50</v>
@@ -922,9 +926,7 @@
       <c r="Q4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="R4" s="3"/>
       <c r="S4" s="3" t="s">
         <v>50</v>
       </c>
@@ -1000,9 +1002,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>50</v>
@@ -1046,14 +1048,14 @@
       <c r="S5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="X5" s="3" t="s">
         <v>50</v>
       </c>
@@ -1118,9 +1120,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>50</v>
@@ -1236,36 +1238,58 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="N7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="Q7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="R7" s="3"/>
+      <c r="R7" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="S7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
+      <c r="T7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3" t="s">
@@ -1295,7 +1319,9 @@
       <c r="AF7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AG7" s="3"/>
+      <c r="AG7" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="AH7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1306,8 +1332,12 @@
       <c r="AK7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="3"/>
+      <c r="AL7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM7" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="AN7" s="4"/>
       <c r="AO7" s="3"/>
       <c r="AP7" s="3"/>
@@ -1326,9 +1356,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1339,9 +1369,7 @@
       <c r="H8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -1352,15 +1380,11 @@
       <c r="Q8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="R8" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="R8" s="3"/>
       <c r="S8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T8" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
@@ -1422,9 +1446,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1518,9 +1542,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1614,9 +1638,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1624,29 +1648,25 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="I11" s="3" t="s">
         <v>50</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
       <c r="Q11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="R11" s="3"/>
+      <c r="R11" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="S11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1654,12 +1674,8 @@
         <v>50</v>
       </c>
       <c r="U11" s="3"/>
-      <c r="V11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
       <c r="X11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1687,27 +1703,19 @@
       <c r="AF11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AG11" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="AG11" s="3"/>
       <c r="AH11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AI11" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="AI11" s="3"/>
       <c r="AJ11" s="3" t="s">
         <v>50</v>
       </c>
       <c r="AK11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AL11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM11" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
       <c r="AN11" s="4"/>
       <c r="AO11" s="3"/>
       <c r="AP11" s="3"/>
@@ -1726,9 +1734,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1741,12 +1749,8 @@
         <v>50</v>
       </c>
       <c r="J12" s="3"/>
-      <c r="K12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
       <c r="M12" s="3" t="s">
         <v>50</v>
       </c>
@@ -1770,8 +1774,12 @@
         <v>50</v>
       </c>
       <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
+      <c r="V12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="X12" s="3" t="s">
         <v>50</v>
       </c>
@@ -1838,9 +1846,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1849,7 +1857,9 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
         <v>50</v>
@@ -1876,7 +1886,9 @@
       <c r="S13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T13" s="3"/>
+      <c r="T13" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
@@ -1946,9 +1958,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1958,12 +1970,16 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="N14" s="3" t="s">
         <v>50</v>
       </c>
@@ -1980,9 +1996,7 @@
       <c r="S14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T14" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
@@ -2013,28 +2027,30 @@
       <c r="AF14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AG14" s="3"/>
+      <c r="AG14" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="AH14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AI14" s="3"/>
+      <c r="AI14" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="AJ14" s="3" t="s">
         <v>50</v>
       </c>
       <c r="AK14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AL14" s="3"/>
-      <c r="AM14" s="3"/>
-      <c r="AN14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AO14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP14" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="AL14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN14" s="4"/>
+      <c r="AO14" s="3"/>
+      <c r="AP14" s="3"/>
       <c r="AQ14" s="3"/>
       <c r="AR14" s="3" t="s">
         <v>50</v>
@@ -2050,9 +2066,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2084,7 +2100,9 @@
       <c r="S15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T15" s="3"/>
+      <c r="T15" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
@@ -2152,7 +2170,113 @@
         <v>50</v>
       </c>
     </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="3"/>
+      <c r="AN16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ16" s="3"/>
+      <c r="AR16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS16" s="3"/>
+      <c r="AT16" s="3"/>
+      <c r="AU16" s="3"/>
+      <c r="AV16" s="3"/>
+      <c r="AW16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX16" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <mergeCells count="1">
+    <mergeCell ref="B1:S1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>